<commit_message>
updated most of the ontology files - still need to add the ners
</commit_message>
<xml_diff>
--- a/resources/EMFOConceptsAndRelationships.xlsx
+++ b/resources/EMFOConceptsAndRelationships.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\divitag2\work\softwareRepos\framework-legacy\01_Sandboxes\850_emfo_utilities\85_01_resources\src\main\resources\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26AA9F6-1C86-44C6-B336-2D30F5DD38E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1BA7AA-A7E2-465C-83F7-2958038ED0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31560" yWindow="645" windowWidth="23970" windowHeight="12870" tabRatio="666" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31560" yWindow="645" windowWidth="23970" windowHeight="12870" tabRatio="666" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="482">
   <si>
     <t>Output</t>
   </si>
@@ -2068,9 +2068,6 @@
     <t>UMLS</t>
   </si>
   <si>
-    <t>Temporal nature</t>
-  </si>
-  <si>
     <t>EMFO_C972246</t>
   </si>
   <si>
@@ -2083,9 +2080,6 @@
     <t>EMFO_C374881</t>
   </si>
   <si>
-    <t>EMFO_C498790</t>
-  </si>
-  <si>
     <t>EMFO_C191549</t>
   </si>
   <si>
@@ -2353,13 +2347,13 @@
     <t>behavior(1)</t>
   </si>
   <si>
-    <t>tmp_id</t>
-  </si>
-  <si>
     <t>#EMFO_C016694</t>
   </si>
   <si>
     <t xml:space="preserve">See the file OntologyTopLevelDefinitions.xlsx </t>
+  </si>
+  <si>
+    <t>#EMFO_C498790</t>
   </si>
 </sst>
 </file>
@@ -3542,11 +3536,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T98"/>
+  <dimension ref="A1:T97"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3597,43 +3591,43 @@
     </row>
     <row r="2" spans="1:20" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B2" s="68" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D2" s="69"/>
     </row>
     <row r="3" spans="1:20" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B3" s="68" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C3" s="68" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D3" s="69"/>
     </row>
     <row r="4" spans="1:20" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="68" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B4" s="68" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C4" s="68" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D4" s="69"/>
     </row>
     <row r="5" spans="1:20" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B5" s="68" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C5" s="68" t="s">
         <v>237</v>
@@ -3645,10 +3639,10 @@
     </row>
     <row r="6" spans="1:20" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="68" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B6" s="68" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C6" s="68" t="s">
         <v>237</v>
@@ -3657,33 +3651,33 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>252</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D7" s="63" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>465</v>
+        <v>0</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>0</v>
@@ -3700,7 +3694,7 @@
         <v>237</v>
       </c>
       <c r="D9" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>7</v>
@@ -3717,10 +3711,10 @@
         <v>0</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>7</v>
@@ -3751,10 +3745,10 @@
         <v>47</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="D11" s="67" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>5</v>
@@ -3785,10 +3779,10 @@
         <v>254</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>237</v>
+        <v>21</v>
       </c>
       <c r="D12" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>8</v>
@@ -3819,10 +3813,10 @@
         <v>48</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>237</v>
+        <v>21</v>
       </c>
       <c r="D13" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>8</v>
@@ -3853,7 +3847,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>473</v>
+        <v>47</v>
       </c>
       <c r="D14" s="67"/>
       <c r="F14" s="45" t="s">
@@ -3882,10 +3876,10 @@
         <v>49</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D15" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>8</v>
@@ -3919,7 +3913,7 @@
         <v>49</v>
       </c>
       <c r="D16" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>8</v>
@@ -3953,7 +3947,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="67" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>5</v>
@@ -3987,7 +3981,7 @@
         <v>3</v>
       </c>
       <c r="D18" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>8</v>
@@ -4021,7 +4015,7 @@
         <v>3</v>
       </c>
       <c r="D19" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>8</v>
@@ -4055,7 +4049,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>8</v>
@@ -4089,7 +4083,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>8</v>
@@ -4123,7 +4117,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>8</v>
@@ -4157,7 +4151,7 @@
         <v>3</v>
       </c>
       <c r="D23" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>8</v>
@@ -4191,7 +4185,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>8</v>
@@ -4225,7 +4219,7 @@
         <v>3</v>
       </c>
       <c r="D25" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>8</v>
@@ -4259,7 +4253,7 @@
         <v>21</v>
       </c>
       <c r="D26" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>8</v>
@@ -4293,7 +4287,7 @@
         <v>59</v>
       </c>
       <c r="D27" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>8</v>
@@ -4327,7 +4321,7 @@
         <v>59</v>
       </c>
       <c r="D28" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>8</v>
@@ -4361,7 +4355,7 @@
         <v>59</v>
       </c>
       <c r="D29" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>8</v>
@@ -4395,7 +4389,7 @@
         <v>59</v>
       </c>
       <c r="D30" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>8</v>
@@ -4429,7 +4423,7 @@
         <v>235</v>
       </c>
       <c r="D31" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>8</v>
@@ -4492,7 +4486,7 @@
         <v>21</v>
       </c>
       <c r="D33" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>8</v>
@@ -4526,7 +4520,7 @@
         <v>62</v>
       </c>
       <c r="D34" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>8</v>
@@ -4589,7 +4583,7 @@
         <v>237</v>
       </c>
       <c r="D36" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>7</v>
@@ -4652,7 +4646,7 @@
         <v>62</v>
       </c>
       <c r="D38" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>8</v>
@@ -4686,7 +4680,7 @@
         <v>64</v>
       </c>
       <c r="D39" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>8</v>
@@ -4720,7 +4714,7 @@
         <v>69</v>
       </c>
       <c r="D40" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>8</v>
@@ -4754,7 +4748,7 @@
         <v>68</v>
       </c>
       <c r="D41" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>7</v>
@@ -4788,7 +4782,7 @@
         <v>68</v>
       </c>
       <c r="D42" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>8</v>
@@ -4822,7 +4816,7 @@
         <v>64</v>
       </c>
       <c r="D43" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>8</v>
@@ -4856,7 +4850,7 @@
         <v>66</v>
       </c>
       <c r="D44" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>7</v>
@@ -4890,7 +4884,7 @@
         <v>66</v>
       </c>
       <c r="D45" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>7</v>
@@ -4924,7 +4918,7 @@
         <v>66</v>
       </c>
       <c r="D46" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>7</v>
@@ -4958,7 +4952,7 @@
         <v>237</v>
       </c>
       <c r="D47" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>8</v>
@@ -4989,7 +4983,7 @@
         <v>35</v>
       </c>
       <c r="D48" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>7</v>
@@ -5023,7 +5017,7 @@
         <v>237</v>
       </c>
       <c r="D49" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>7</v>
@@ -5057,7 +5051,7 @@
         <v>21</v>
       </c>
       <c r="D50" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>7</v>
@@ -5091,7 +5085,7 @@
         <v>75</v>
       </c>
       <c r="D51" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>7</v>
@@ -5125,7 +5119,7 @@
         <v>75</v>
       </c>
       <c r="D52" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>7</v>
@@ -5159,7 +5153,7 @@
         <v>21</v>
       </c>
       <c r="D53" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>7</v>
@@ -5193,7 +5187,7 @@
         <v>76</v>
       </c>
       <c r="D54" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E54" s="7" t="s">
         <v>7</v>
@@ -5227,7 +5221,7 @@
         <v>76</v>
       </c>
       <c r="D55" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>7</v>
@@ -5261,7 +5255,7 @@
         <v>77</v>
       </c>
       <c r="D56" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>7</v>
@@ -5295,7 +5289,7 @@
         <v>77</v>
       </c>
       <c r="D57" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>7</v>
@@ -5329,7 +5323,7 @@
         <v>77</v>
       </c>
       <c r="D58" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>7</v>
@@ -5363,7 +5357,7 @@
         <v>76</v>
       </c>
       <c r="D59" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>7</v>
@@ -5397,7 +5391,7 @@
         <v>82</v>
       </c>
       <c r="D60" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>7</v>
@@ -5431,7 +5425,7 @@
         <v>82</v>
       </c>
       <c r="D61" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E61" s="7" t="s">
         <v>7</v>
@@ -5465,7 +5459,7 @@
         <v>82</v>
       </c>
       <c r="D62" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>7</v>
@@ -5499,7 +5493,7 @@
         <v>21</v>
       </c>
       <c r="D63" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>7</v>
@@ -5533,7 +5527,7 @@
         <v>86</v>
       </c>
       <c r="D64" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>7</v>
@@ -5567,7 +5561,7 @@
         <v>86</v>
       </c>
       <c r="D65" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>7</v>
@@ -5598,10 +5592,10 @@
         <v>39</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D66" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>7</v>
@@ -5635,7 +5629,7 @@
         <v>39</v>
       </c>
       <c r="D67" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>7</v>
@@ -5669,7 +5663,7 @@
         <v>39</v>
       </c>
       <c r="D68" s="66" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>7</v>
@@ -5703,7 +5697,7 @@
         <v>235</v>
       </c>
       <c r="D70" s="65" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>224</v>
@@ -5720,7 +5714,7 @@
         <v>249</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D71" s="65"/>
       <c r="E71" s="6" t="s">
@@ -5732,16 +5726,16 @@
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>237</v>
       </c>
       <c r="D72" s="66" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E72" s="7" t="s">
         <v>227</v>
@@ -5752,16 +5746,16 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B73" s="48" t="s">
         <v>238</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D73" s="65" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>239</v>
@@ -5772,16 +5766,16 @@
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="45" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B74" s="49" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C74" s="45" t="s">
         <v>219</v>
       </c>
       <c r="D74" s="64" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E74" s="45" t="s">
         <v>241</v>
@@ -5792,16 +5786,16 @@
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B75" s="48" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>219</v>
       </c>
       <c r="D75" s="65" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>239</v>
@@ -5812,10 +5806,10 @@
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="60" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>49</v>
@@ -5829,10 +5823,10 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="60" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>49</v>
@@ -5846,10 +5840,10 @@
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>49</v>
@@ -5860,10 +5854,10 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>68</v>
@@ -5877,10 +5871,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>391</v>
+        <v>481</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>37</v>
@@ -5894,10 +5888,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>49</v>
@@ -5911,10 +5905,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>49</v>
@@ -5928,10 +5922,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>69</v>
@@ -5945,7 +5939,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>64</v>
@@ -5962,10 +5956,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>64</v>
@@ -5979,10 +5973,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>49</v>
@@ -5996,10 +5990,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>49</v>
@@ -6013,10 +6007,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>64</v>
@@ -6030,10 +6024,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>64</v>
@@ -6047,10 +6041,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>64</v>
@@ -6064,10 +6058,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>59</v>
@@ -6081,10 +6075,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>59</v>
@@ -6098,10 +6092,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>59</v>
@@ -6115,10 +6109,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>59</v>
@@ -6132,10 +6126,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>59</v>
@@ -6147,30 +6141,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>481</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>59</v>
-      </c>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B97" s="9"/>
+      <c r="C97" s="9"/>
       <c r="E97" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B98" s="9"/>
-      <c r="C98" s="9"/>
-      <c r="E98" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F98" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7185,7 +7162,7 @@
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="44"/>
       <c r="B65" s="44" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C65" s="44"/>
     </row>
@@ -7391,7 +7368,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7399,10 +7376,10 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E3" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7413,10 +7390,10 @@
         <v>157</v>
       </c>
       <c r="E4" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7427,10 +7404,10 @@
         <v>158</v>
       </c>
       <c r="E5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7441,7 +7418,7 @@
         <v>159</v>
       </c>
       <c r="E6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -7449,10 +7426,10 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E7" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -7463,7 +7440,7 @@
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -7474,10 +7451,10 @@
         <v>160</v>
       </c>
       <c r="E9" t="s">
+        <v>420</v>
+      </c>
+      <c r="F9" t="s">
         <v>422</v>
-      </c>
-      <c r="F9" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -7488,10 +7465,10 @@
         <v>161</v>
       </c>
       <c r="E10" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F10" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -7502,43 +7479,43 @@
         <v>162</v>
       </c>
       <c r="E11" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>407</v>
+      </c>
+      <c r="B12" t="s">
+        <v>408</v>
+      </c>
+      <c r="E12" t="s">
         <v>409</v>
-      </c>
-      <c r="B12" t="s">
-        <v>410</v>
-      </c>
-      <c r="E12" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B14" t="s">
         <v>257</v>
       </c>
       <c r="E14" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F14" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -8218,7 +8195,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E21" s="44"/>
       <c r="F21" s="51"/>
@@ -9032,7 +9009,7 @@
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E46" s="44"/>
       <c r="F46" s="51"/>
@@ -9516,7 +9493,7 @@
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E61" s="44"/>
       <c r="F61" s="51"/>
@@ -9752,7 +9729,7 @@
         <v>28</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D69" s="17" t="s">
         <v>235</v>
@@ -9776,7 +9753,7 @@
         <v>64</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D70" s="17" t="s">
         <v>219</v>
@@ -9800,10 +9777,10 @@
         <v>35</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E71" s="55" t="s">
         <v>28</v>
@@ -9824,7 +9801,7 @@
         <v>65</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D72" s="17" t="s">
         <v>238</v>
@@ -9848,10 +9825,10 @@
         <v>49</v>
       </c>
       <c r="C73" s="47" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D73" s="46" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E73" s="54" t="s">
         <v>0</v>
@@ -9872,10 +9849,10 @@
         <v>69</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D74" s="46" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E74" s="54" t="s">
         <v>0</v>
@@ -10350,7 +10327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F53A5C-C61C-46C4-AC07-17A8415AFB31}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed: changed the direction of the functioning realizes function to functioning -> realized_by function
</commit_message>
<xml_diff>
--- a/resources/EMFOConceptsAndRelationships.xlsx
+++ b/resources/EMFOConceptsAndRelationships.xlsx
@@ -1,31 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\divitag2\work\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\softwareRepos\EcologicalMentalFunctioningOntology\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1FDB21-E6E2-4AD6-8F1A-930D8D0F274E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96364F9D-A66E-4332-BE1A-55702F8AEBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="930" windowWidth="34875" windowHeight="18000" tabRatio="666" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="16845" windowWidth="35055" windowHeight="19335" tabRatio="666" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
     <sheet name="EMFO_Picture" sheetId="22" r:id="rId2"/>
     <sheet name="Definitions" sheetId="17" r:id="rId3"/>
-    <sheet name="Dictionary" sheetId="18" r:id="rId4"/>
-    <sheet name="References" sheetId="19" r:id="rId5"/>
-    <sheet name="Sources" sheetId="15" r:id="rId6"/>
-    <sheet name="Relations" sheetId="4" r:id="rId7"/>
-    <sheet name="Relationships" sheetId="2" r:id="rId8"/>
-    <sheet name="Technical Notes" sheetId="14" r:id="rId9"/>
+    <sheet name="References" sheetId="19" r:id="rId4"/>
+    <sheet name="Sources" sheetId="15" r:id="rId5"/>
+    <sheet name="Relations" sheetId="4" r:id="rId6"/>
+    <sheet name="Relationships" sheetId="2" r:id="rId7"/>
+    <sheet name="Technical Notes" sheetId="14" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classes!$A$1:$G$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Relationships!$P$20:$P$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Relationships!$P$20:$P$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2483" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2481" uniqueCount="945">
   <si>
     <t>Output</t>
   </si>
@@ -4685,67 +4684,6 @@
     <t>EMFO_D643924</t>
   </si>
   <si>
-    <t>Theoretical definition</t>
-  </si>
-  <si>
-    <r>
-      <t>Theoretical definitions are basic dictionary definitions. They are frequently called </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>constitutive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>conceptual</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> definitions. A theoretical definition gives meaning to the concept or construct under investigation. It should distinguish it from all other concepts or constructs</t>
-    </r>
-  </si>
-  <si>
-    <t>Operational definition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operational definitions provide an observable way to measure or apply the concept.  In this case, the operational defintion will be how each concept in the ontology is defined specifically as it relates to it's role in mental functionioning.   </t>
-  </si>
-  <si>
-    <t>Scoring of agreement with the operational definitons</t>
-  </si>
-  <si>
-    <t>0 = disagree
-1 = agree
-blank = not yet voted
-something else =  Please use comments section for explaination</t>
-  </si>
-  <si>
     <t>“Environment.” Merriam-Webster.com Dictionary, Merriam-Webster, https://www.merriam-webster.com/dictionary/environment. Accessed 6 Apr. 2022.</t>
   </si>
   <si>
@@ -4932,14 +4870,29 @@
     <t>EMFO_C592475</t>
   </si>
   <si>
-    <t xml:space="preserve">This is version 2025-05-16 </t>
+    <t>This is version 2025-07-23</t>
+  </si>
+  <si>
+    <t>realized-by</t>
+  </si>
+  <si>
+    <t>BFO_0000054</t>
+  </si>
+  <si>
+    <t>Paraphrase of elucidation: a relation between a realizable entity and a process, where there is some material entity that is bearer of the realizable entity and participates in the process, and the realizable entity comes to be realized in the course of the process</t>
+  </si>
+  <si>
+    <t>realized_by</t>
+  </si>
+  <si>
+    <t>realizes_by</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5221,19 +5174,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -5776,7 +5716,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5970,18 +5910,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="10" xfId="7" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="6" applyBorder="1"/>
@@ -6064,23 +5998,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>96307</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>27385</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>48266</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13E8E0D9-B306-8B9B-7C9C-FACFF31B3C62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4289CAC-E3E5-12A1-2A80-D6A6CB2C9C49}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6102,8 +6036,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="96307" y="2933700"/>
-          <a:ext cx="18201218" cy="10238185"/>
+          <a:off x="619125" y="190500"/>
+          <a:ext cx="15678150" cy="8811266"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6538,7 +6472,7 @@
         <v>560</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>930</v>
+        <v>924</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>218</v>
@@ -6606,7 +6540,7 @@
         <v>30</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="K11"/>
       <c r="L11"/>
@@ -6710,12 +6644,12 @@
     </row>
     <row r="15" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>942</v>
+        <v>936</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C15" s="117" t="s">
+      <c r="C15" s="115" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="48"/>
@@ -6723,7 +6657,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>902</v>
+        <v>896</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -6741,7 +6675,7 @@
     </row>
     <row r="16" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>942</v>
+        <v>936</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>217</v>
@@ -6749,15 +6683,15 @@
       <c r="C16" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="D16" s="115"/>
-      <c r="E16" s="116" t="s">
+      <c r="D16" s="113"/>
+      <c r="E16" s="114" t="s">
         <v>209</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -6810,22 +6744,22 @@
       <c r="T17" s="4"/>
     </row>
     <row r="18" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="118" t="s">
+      <c r="A18" s="116" t="s">
         <v>439</v>
       </c>
-      <c r="B18" s="118" t="s">
+      <c r="B18" s="116" t="s">
         <v>428</v>
       </c>
-      <c r="C18" s="118" t="s">
+      <c r="C18" s="116" t="s">
         <v>437</v>
       </c>
-      <c r="D18" s="119"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118" t="s">
+      <c r="D18" s="117"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="G18" s="118" t="s">
-        <v>903</v>
+      <c r="G18" s="116" t="s">
+        <v>897</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -6859,7 +6793,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -7021,7 +6955,7 @@
       <c r="C25" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="115"/>
+      <c r="D25" s="113"/>
       <c r="F25" s="31" t="s">
         <v>0</v>
       </c>
@@ -7052,7 +6986,7 @@
       <c r="C26" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="D26" s="115"/>
+      <c r="D26" s="113"/>
       <c r="E26" s="5" t="s">
         <v>211</v>
       </c>
@@ -7226,7 +7160,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>905</v>
+        <v>899</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
@@ -7279,26 +7213,26 @@
       <c r="T32" s="4"/>
     </row>
     <row r="33" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="116" t="s">
+      <c r="A33" s="114" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="116" t="s">
+      <c r="B33" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="116" t="s">
+      <c r="C33" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="115" t="s">
+      <c r="D33" s="113" t="s">
         <v>381</v>
       </c>
-      <c r="E33" s="116" t="s">
+      <c r="E33" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="116" t="s">
+      <c r="F33" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="G33" s="116" t="s">
-        <v>906</v>
+      <c r="G33" s="114" t="s">
+        <v>900</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -7622,7 +7556,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
@@ -8108,22 +8042,22 @@
       <c r="A62" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B62" s="116" t="s">
+      <c r="B62" s="114" t="s">
         <v>54</v>
       </c>
-      <c r="C62" s="116" t="s">
+      <c r="C62" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="D62" s="115"/>
-      <c r="E62" s="116"/>
-      <c r="F62" s="116" t="s">
+      <c r="D62" s="113"/>
+      <c r="E62" s="114"/>
+      <c r="F62" s="114" t="s">
         <v>24</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>417</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>911</v>
+        <v>905</v>
       </c>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
@@ -8158,10 +8092,10 @@
         <v>24</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -8196,10 +8130,10 @@
         <v>24</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
@@ -8305,10 +8239,10 @@
         <v>24</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
@@ -8374,10 +8308,10 @@
         <v>24</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
@@ -8453,7 +8387,7 @@
         <v>436</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="4"/>
@@ -8769,7 +8703,7 @@
     </row>
     <row r="80" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>919</v>
+        <v>913</v>
       </c>
       <c r="D80" s="45" t="s">
         <v>478</v>
@@ -8844,7 +8778,7 @@
         <v>495</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
@@ -8861,10 +8795,10 @@
     </row>
     <row r="83" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>943</v>
+        <v>937</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>922</v>
+        <v>916</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>29</v>
@@ -9096,7 +9030,7 @@
         <v>417</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
@@ -9128,7 +9062,7 @@
         <v>449</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>914</v>
+        <v>908</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>423</v>
@@ -9152,7 +9086,7 @@
         <v>450</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>915</v>
+        <v>909</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>423</v>
@@ -9375,7 +9309,7 @@
         <v>30</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
@@ -9588,7 +9522,7 @@
         <v>417</v>
       </c>
       <c r="H109" s="4" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="I109" s="4"/>
       <c r="J109" s="4"/>
@@ -10001,10 +9935,10 @@
         <v>30</v>
       </c>
       <c r="G120" s="4" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="H120" s="4" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="I120" s="4"/>
       <c r="J120" s="4"/>
@@ -10059,7 +9993,7 @@
     </row>
     <row r="122" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>944</v>
+        <v>938</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>488</v>
@@ -10443,7 +10377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB80F22D-8378-4BC5-BBF6-7BBCD372B323}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AI25" sqref="AI25"/>
     </sheetView>
   </sheetViews>
@@ -10458,7 +10392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196853EE-79FD-4CFA-83CE-DB26EE5C20FD}">
   <dimension ref="A1:W120"/>
   <sheetViews>
-    <sheetView topLeftCell="B20" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+    <sheetView topLeftCell="B23" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
       <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
@@ -13750,60 +13684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE6BE49-537F-4AFC-8AC4-7CAD3A8967E1}">
-  <dimension ref="A2:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.7109375" style="110" customWidth="1"/>
-    <col min="2" max="2" width="64.140625" style="110" customWidth="1"/>
-    <col min="3" max="16384" width="8.7109375" style="110"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:2" ht="48" x14ac:dyDescent="0.25">
-      <c r="A2" s="110" t="s">
-        <v>878</v>
-      </c>
-      <c r="B2" s="111" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="36" x14ac:dyDescent="0.25">
-      <c r="A3" s="110" t="s">
-        <v>880</v>
-      </c>
-      <c r="B3" s="111" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="112" t="s">
-        <v>882</v>
-      </c>
-      <c r="B4" s="112" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="110" t="s">
-        <v>478</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935EC933-5237-4B6B-9FAA-5370FFD1B9EC}">
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13813,72 +13698,72 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="112" t="s">
-        <v>886</v>
+      <c r="A3" s="110" t="s">
+        <v>880</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="113" t="s">
-        <v>888</v>
+      <c r="A5" s="111" t="s">
+        <v>882</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>897</v>
+        <v>891</v>
       </c>
     </row>
   </sheetData>
@@ -13886,7 +13771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC84FB6-CA19-4234-BB2F-E661E09ED822}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -14027,12 +13912,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D798B18-C5BD-476F-9FF2-CDB45434B078}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14201,7 +14086,7 @@
         <v>402</v>
       </c>
       <c r="D9" t="s">
-        <v>926</v>
+        <v>920</v>
       </c>
       <c r="E9" t="s">
         <v>371</v>
@@ -14295,110 +14180,122 @@
         <v>480</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>940</v>
+      </c>
+      <c r="B15" t="s">
+        <v>941</v>
+      </c>
+      <c r="C15" t="s">
+        <v>477</v>
+      </c>
+      <c r="D15" t="s">
+        <v>217</v>
+      </c>
+      <c r="E15" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>470</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>471</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>217</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>477</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E16" s="59" t="s">
         <v>472</v>
       </c>
-      <c r="F15" s="59" t="s">
+      <c r="F16" s="59" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>474</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>475</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>405</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>218</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E17" s="59" t="s">
         <v>476</v>
       </c>
-      <c r="F16" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>907</v>
-      </c>
-      <c r="B17" t="s">
-        <v>927</v>
-      </c>
-      <c r="C17" t="s">
-        <v>481</v>
-      </c>
-      <c r="D17" t="s">
-        <v>405</v>
-      </c>
-      <c r="E17" t="s">
-        <v>499</v>
-      </c>
       <c r="F17" t="s">
-        <v>500</v>
+        <v>919</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>901</v>
+      </c>
+      <c r="B18" t="s">
         <v>921</v>
       </c>
-      <c r="B18" t="s">
-        <v>928</v>
-      </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>481</v>
       </c>
       <c r="D18" t="s">
-        <v>437</v>
-      </c>
-      <c r="E18" s="58" t="s">
-        <v>377</v>
+        <v>405</v>
+      </c>
+      <c r="E18" t="s">
+        <v>499</v>
+      </c>
+      <c r="F18" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>909</v>
+        <v>915</v>
       </c>
       <c r="B19" t="s">
-        <v>929</v>
+        <v>922</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>437</v>
       </c>
       <c r="E19" s="58" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>903</v>
+      </c>
+      <c r="B20" t="s">
+        <v>923</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="58" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="37"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>478</v>
       </c>
     </row>
@@ -14409,6 +14306,11 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>478</v>
       </c>
     </row>
@@ -14418,12 +14320,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B15F685-1533-4446-BC92-30DBE05F964F}">
   <dimension ref="A1:U115"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14455,10 +14357,10 @@
         <v>340</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>898</v>
+        <v>892</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>899</v>
+        <v>893</v>
       </c>
       <c r="M1" s="38"/>
       <c r="N1" s="38"/>
@@ -14485,7 +14387,7 @@
       <c r="E2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="114" t="s">
+      <c r="F2" s="112" t="s">
         <v>417</v>
       </c>
       <c r="G2" t="s">
@@ -14583,7 +14485,7 @@
         <v>437</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>900</v>
+        <v>894</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>0</v>
@@ -14612,7 +14514,7 @@
     </row>
     <row r="6" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>931</v>
+        <v>925</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>428</v>
@@ -15255,7 +15157,7 @@
         <v>498</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>907</v>
+        <v>901</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>435</v>
@@ -15266,7 +15168,7 @@
         <v>417</v>
       </c>
       <c r="H24" t="s">
-        <v>908</v>
+        <v>902</v>
       </c>
       <c r="I24"/>
       <c r="J24"/>
@@ -15305,7 +15207,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="B26" s="32" t="s">
         <v>429</v>
@@ -15326,7 +15228,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>933</v>
+        <v>927</v>
       </c>
       <c r="B27" s="32" t="s">
         <v>431</v>
@@ -15347,7 +15249,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>934</v>
+        <v>928</v>
       </c>
       <c r="B28" s="32" t="s">
         <v>432</v>
@@ -15437,7 +15339,7 @@
         <v>24</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>909</v>
+        <v>903</v>
       </c>
       <c r="D32" s="65" t="s">
         <v>30</v>
@@ -15450,7 +15352,7 @@
         <v>417</v>
       </c>
       <c r="H32" t="s">
-        <v>910</v>
+        <v>904</v>
       </c>
       <c r="I32"/>
       <c r="J32"/>
@@ -15467,7 +15369,7 @@
     </row>
     <row r="33" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>935</v>
+        <v>929</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>54</v>
@@ -16111,7 +16013,7 @@
     </row>
     <row r="51" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>936</v>
+        <v>930</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>61</v>
@@ -16119,7 +16021,7 @@
       <c r="C51" s="18" t="s">
         <v>470</v>
       </c>
-      <c r="D51" s="117" t="s">
+      <c r="D51" s="115" t="s">
         <v>40</v>
       </c>
       <c r="E51" t="s">
@@ -16229,7 +16131,7 @@
     </row>
     <row r="55" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="53" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="B55" s="53" t="s">
         <v>26</v>
@@ -16243,8 +16145,8 @@
       <c r="E55" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="F55" s="120" t="s">
-        <v>916</v>
+      <c r="F55" s="118" t="s">
+        <v>910</v>
       </c>
       <c r="G55" s="58"/>
       <c r="H55" s="58"/>
@@ -16284,7 +16186,7 @@
         <v>417</v>
       </c>
       <c r="H56" s="68" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="I56"/>
       <c r="J56"/>
@@ -16445,7 +16347,7 @@
     </row>
     <row r="61" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>937</v>
+        <v>931</v>
       </c>
       <c r="B61" s="17" t="s">
         <v>29</v>
@@ -16454,7 +16356,7 @@
         <v>497</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>922</v>
+        <v>916</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>24</v>
@@ -16526,7 +16428,7 @@
         <v>24</v>
       </c>
       <c r="F63" s="68" t="s">
-        <v>923</v>
+        <v>917</v>
       </c>
       <c r="P63"/>
     </row>
@@ -16556,7 +16458,7 @@
     </row>
     <row r="65" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
-        <v>938</v>
+        <v>932</v>
       </c>
       <c r="B65" s="16" t="s">
         <v>56</v>
@@ -16564,7 +16466,7 @@
       <c r="C65" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D65" s="122" t="s">
+      <c r="D65" s="120" t="s">
         <v>81</v>
       </c>
       <c r="E65" s="16" t="s">
@@ -16575,7 +16477,7 @@
       </c>
       <c r="G65"/>
       <c r="H65" s="68" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="I65"/>
       <c r="J65"/>
@@ -16699,7 +16601,7 @@
         <v>61</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>470</v>
+        <v>943</v>
       </c>
       <c r="D69" s="13" t="s">
         <v>40</v>
@@ -16712,7 +16614,7 @@
         <v>417</v>
       </c>
       <c r="H69" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="I69"/>
       <c r="J69"/>
@@ -16735,7 +16637,7 @@
         <v>551</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>470</v>
+        <v>944</v>
       </c>
       <c r="D70" s="12" t="s">
         <v>217</v>
@@ -16748,7 +16650,7 @@
         <v>417</v>
       </c>
       <c r="H70" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="I70"/>
       <c r="J70"/>
@@ -16771,7 +16673,7 @@
         <v>551</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>470</v>
+        <v>944</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>421</v>
@@ -16784,7 +16686,7 @@
         <v>417</v>
       </c>
       <c r="H71" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="I71"/>
       <c r="J71"/>
@@ -16820,7 +16722,7 @@
         <v>417</v>
       </c>
       <c r="H72" t="s">
-        <v>924</v>
+        <v>918</v>
       </c>
       <c r="I72"/>
       <c r="J72"/>
@@ -16846,7 +16748,7 @@
         <v>468</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>922</v>
+        <v>916</v>
       </c>
       <c r="E73" s="49"/>
       <c r="F73" t="s">
@@ -17092,7 +16994,7 @@
     </row>
     <row r="82" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
-        <v>939</v>
+        <v>933</v>
       </c>
       <c r="B82" s="20" t="s">
         <v>78</v>
@@ -17486,7 +17388,7 @@
         <v>417</v>
       </c>
       <c r="H93" t="s">
-        <v>920</v>
+        <v>914</v>
       </c>
       <c r="I93"/>
       <c r="J93"/>
@@ -17525,7 +17427,7 @@
         <v>417</v>
       </c>
       <c r="H94" t="s">
-        <v>920</v>
+        <v>914</v>
       </c>
       <c r="I94"/>
       <c r="J94"/>
@@ -17580,7 +17482,7 @@
     </row>
     <row r="96" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="20" t="s">
-        <v>940</v>
+        <v>934</v>
       </c>
       <c r="B96" s="21" t="s">
         <v>68</v>
@@ -17708,7 +17610,7 @@
         <v>417</v>
       </c>
       <c r="H99" t="s">
-        <v>918</v>
+        <v>912</v>
       </c>
       <c r="I99"/>
       <c r="J99"/>
@@ -17783,15 +17685,15 @@
     </row>
     <row r="102" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="B102" s="21" t="s">
         <v>68</v>
       </c>
       <c r="C102" s="22" t="s">
-        <v>921</v>
-      </c>
-      <c r="D102" s="117" t="s">
+        <v>915</v>
+      </c>
+      <c r="D102" s="115" t="s">
         <v>421</v>
       </c>
       <c r="E102"/>
@@ -17825,10 +17727,10 @@
       <c r="D104" s="27" t="s">
         <v>231</v>
       </c>
-      <c r="E104" s="122" t="s">
+      <c r="E104" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="F104" s="121"/>
+      <c r="F104" s="119"/>
       <c r="G104"/>
       <c r="H104"/>
       <c r="I104"/>
@@ -18037,19 +17939,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F53A5C-C61C-46C4-AC07-17A8415AFB31}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>945</v>
+        <v>939</v>
       </c>
     </row>
   </sheetData>
@@ -18058,6 +17960,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="0c85289e-a0a4-4193-8a36-83840327cccf" xsi:nil="true"/>
@@ -18066,15 +17977,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18333,6 +18235,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4B4AC16-F988-4D41-8F01-205FCE01B916}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{084C8915-1C39-4800-8751-2F69F55F51E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -18345,14 +18255,6 @@
     <ds:schemaRef ds:uri="0c85289e-a0a4-4193-8a36-83840327cccf"/>
     <ds:schemaRef ds:uri="48f24ce9-3fee-408f-adaa-6c70c8fcad88"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4B4AC16-F988-4D41-8F01-205FCE01B916}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>